<commit_message>
Added new logic for card click tests
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-commonobj.xlsx
+++ b/test-data/webanalytics-commonobj.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5112B773-5A3F-407C-9270-8DF2B8EF2488}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C2CA8A90-FECE-4344-A386-64B28161390E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Path</t>
   </si>
   <si>
     <t>ContentType</t>
+  </si>
+  <si>
+    <t>CardPos</t>
   </si>
   <si>
     <t>/</t>
@@ -101,11 +104,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,7 +424,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F2B56E1-BA35-4071-8CAC-1CCCC51E0A7D}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -435,7 +439,7 @@
     <col min="5" max="5" width="31" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,30 +447,36 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned and added more tests for CardClick_Test
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-commonobj.xlsx
+++ b/test-data/webanalytics-commonobj.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C2CA8A90-FECE-4344-A386-64B28161390E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D55412C7-BCC2-4A04-A960-06CCD385C394}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="HomeLandingCards" sheetId="10" r:id="rId1"/>
+    <sheet name="HomeLandingTopicCards" sheetId="10" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
   <si>
     <t>Path</t>
   </si>
@@ -55,6 +55,66 @@
   </si>
   <si>
     <t>.feature-primary .feature-card h3</t>
+  </si>
+  <si>
+    <t>Guide</t>
+  </si>
+  <si>
+    <t>.guide-card .card h2</t>
+  </si>
+  <si>
+    <t>.multimedia div[class*=feature-card] h3</t>
+  </si>
+  <si>
+    <t>Multimedia</t>
+  </si>
+  <si>
+    <t>.guide-card .card h2  + ul li a</t>
+  </si>
+  <si>
+    <t>Thumbnail</t>
+  </si>
+  <si>
+    <t>.card-thumbnail h3 a</t>
+  </si>
+  <si>
+    <t>Landing</t>
+  </si>
+  <si>
+    <t>/about-cancer</t>
+  </si>
+  <si>
+    <t>SecondaryFeature</t>
+  </si>
+  <si>
+    <t>.feature-secondary .feature-card h3</t>
+  </si>
+  <si>
+    <t>/about-nci/organization/crchd</t>
+  </si>
+  <si>
+    <t>SlottedTopicCard</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>.topic-feature .feature-card a h3</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment</t>
+  </si>
+  <si>
+    <t>InlineCard</t>
+  </si>
+  <si>
+    <t>#cgvBody .feature-card a h3</t>
+  </si>
+  <si>
+    <t>/espanol/cancer</t>
+  </si>
+  <si>
+    <t>/espanol</t>
   </si>
 </sst>
 </file>
@@ -424,19 +484,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F2B56E1-BA35-4071-8CAC-1CCCC51E0A7D}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -449,11 +509,11 @@
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>2</v>
@@ -477,6 +537,226 @@
       </c>
       <c r="F2" s="4">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added megamenu data sheet
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-commonobj.xlsx
+++ b/test-data/webanalytics-commonobj.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D55412C7-BCC2-4A04-A960-06CCD385C394}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{01C1BA8A-62DF-4E4B-8897-4F2CE423009F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HomeLandingTopicCards" sheetId="10" r:id="rId1"/>
+    <sheet name="MegaMenuInfo" sheetId="11" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="35">
   <si>
     <t>Path</t>
   </si>
@@ -115,6 +116,21 @@
   </si>
   <si>
     <t>/espanol</t>
+  </si>
+  <si>
+    <t>LinkName</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>/espanol/tipos</t>
+  </si>
+  <si>
+    <t>english</t>
+  </si>
+  <si>
+    <t>spanish</t>
   </si>
 </sst>
 </file>
@@ -486,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F2B56E1-BA35-4071-8CAC-1CCCC51E0A7D}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,4 +779,50 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0546EB62-9EAA-40B6-9895-47102C6D888C}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added data method with args for MegaMenu test
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-commonobj.xlsx
+++ b/test-data/webanalytics-commonobj.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B9EAB2BB-3025-4AD2-A5BE-819DA78ACD49}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F3F30EA4-B067-4AB0-8416-FB47055DD1F2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="43">
   <si>
     <t>Path</t>
   </si>
@@ -118,9 +118,6 @@
     <t>/espanol</t>
   </si>
   <si>
-    <t>LinkName</t>
-  </si>
-  <si>
     <t>Language</t>
   </si>
   <si>
@@ -131,6 +128,33 @@
   </si>
   <si>
     <t>spanish</t>
+  </si>
+  <si>
+    <t>NavGroup</t>
+  </si>
+  <si>
+    <t>SubNavGroup</t>
+  </si>
+  <si>
+    <t>ListItem</t>
+  </si>
+  <si>
+    <t>Tipos de cáncer</t>
+  </si>
+  <si>
+    <t>Tipos comunes de cáncer</t>
+  </si>
+  <si>
+    <t>Linfoma</t>
+  </si>
+  <si>
+    <t>About Cancer</t>
+  </si>
+  <si>
+    <t>Understanding Cancer</t>
+  </si>
+  <si>
+    <t>Cancer Statistics</t>
   </si>
 </sst>
 </file>
@@ -783,7 +807,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0546EB62-9EAA-40B6-9895-47102C6D888C}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -793,33 +817,59 @@
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
       <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaning up assertions & link values for mega menu test
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-commonobj.xlsx
+++ b/test-data/webanalytics-commonobj.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F3F30EA4-B067-4AB0-8416-FB47055DD1F2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F2304440-7925-4370-94C3-12659BAA3EEB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -121,9 +121,6 @@
     <t>Language</t>
   </si>
   <si>
-    <t>/espanol/tipos</t>
-  </si>
-  <si>
     <t>english</t>
   </si>
   <si>
@@ -155,6 +152,9 @@
   </si>
   <si>
     <t>Cancer Statistics</t>
+  </si>
+  <si>
+    <t>/espanol/investigacion</t>
   </si>
 </sst>
 </file>
@@ -826,13 +826,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>30</v>
@@ -843,33 +843,33 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
         <v>40</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>41</v>
       </c>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
         <v>37</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>38</v>
       </c>
-      <c r="D3" t="s">
-        <v>39</v>
-      </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rolled back to revision 1353cc2
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-commonobj.xlsx
+++ b/test-data/webanalytics-commonobj.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F2304440-7925-4370-94C3-12659BAA3EEB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D55412C7-BCC2-4A04-A960-06CCD385C394}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HomeLandingTopicCards" sheetId="10" r:id="rId1"/>
-    <sheet name="MegaMenuInfo" sheetId="11" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
   <si>
     <t>Path</t>
   </si>
@@ -116,45 +115,6 @@
   </si>
   <si>
     <t>/espanol</t>
-  </si>
-  <si>
-    <t>Language</t>
-  </si>
-  <si>
-    <t>english</t>
-  </si>
-  <si>
-    <t>spanish</t>
-  </si>
-  <si>
-    <t>NavGroup</t>
-  </si>
-  <si>
-    <t>SubNavGroup</t>
-  </si>
-  <si>
-    <t>ListItem</t>
-  </si>
-  <si>
-    <t>Tipos de cáncer</t>
-  </si>
-  <si>
-    <t>Tipos comunes de cáncer</t>
-  </si>
-  <si>
-    <t>Linfoma</t>
-  </si>
-  <si>
-    <t>About Cancer</t>
-  </si>
-  <si>
-    <t>Understanding Cancer</t>
-  </si>
-  <si>
-    <t>Cancer Statistics</t>
-  </si>
-  <si>
-    <t>/espanol/investigacion</t>
   </si>
 </sst>
 </file>
@@ -526,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F2B56E1-BA35-4071-8CAC-1CCCC51E0A7D}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,76 +763,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0546EB62-9EAA-40B6-9895-47102C6D888C}">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="24.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Re-added page object fixes, mega menu tests
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-commonobj.xlsx
+++ b/test-data/webanalytics-commonobj.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D55412C7-BCC2-4A04-A960-06CCD385C394}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F2304440-7925-4370-94C3-12659BAA3EEB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HomeLandingTopicCards" sheetId="10" r:id="rId1"/>
+    <sheet name="MegaMenuInfo" sheetId="11" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="43">
   <si>
     <t>Path</t>
   </si>
@@ -115,6 +116,45 @@
   </si>
   <si>
     <t>/espanol</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>english</t>
+  </si>
+  <si>
+    <t>spanish</t>
+  </si>
+  <si>
+    <t>NavGroup</t>
+  </si>
+  <si>
+    <t>SubNavGroup</t>
+  </si>
+  <si>
+    <t>ListItem</t>
+  </si>
+  <si>
+    <t>Tipos de cáncer</t>
+  </si>
+  <si>
+    <t>Tipos comunes de cáncer</t>
+  </si>
+  <si>
+    <t>Linfoma</t>
+  </si>
+  <si>
+    <t>About Cancer</t>
+  </si>
+  <si>
+    <t>Understanding Cancer</t>
+  </si>
+  <si>
+    <t>Cancer Statistics</t>
+  </si>
+  <si>
+    <t>/espanol/investigacion</t>
   </si>
 </sst>
 </file>
@@ -486,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F2B56E1-BA35-4071-8CAC-1CCCC51E0A7D}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,4 +803,76 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0546EB62-9EAA-40B6-9895-47102C6D888C}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="24.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added timing / scolling test class
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-commonobj.xlsx
+++ b/test-data/webanalytics-commonobj.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A65FADA8-3362-4B09-A753-36FC70BC6CD0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C008052C-36A0-433E-A971-D1B8E499BF71}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HomeLandingTopicCards" sheetId="10" r:id="rId1"/>
     <sheet name="MegaMenuInfo" sheetId="11" r:id="rId2"/>
+    <sheet name="TimingScroll" sheetId="12" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="49">
   <si>
     <t>Path</t>
   </si>
@@ -158,6 +159,21 @@
   </si>
   <si>
     <t>/PublishedContent/ErrorMessages/PageNotFound.html</t>
+  </si>
+  <si>
+    <t>/news-events</t>
+  </si>
+  <si>
+    <t>/espanol/tipos/vesicula-biliar</t>
+  </si>
+  <si>
+    <t>CTHP</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/types/immunotherapy</t>
+  </si>
+  <si>
+    <t>Article</t>
   </si>
 </sst>
 </file>
@@ -812,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0546EB62-9EAA-40B6-9895-47102C6D888C}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,4 +911,55 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3684BF6F-55B7-48F3-883C-A89530045D73}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
More cleanup: card clicks
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-commonobj.xlsx
+++ b/test-data/webanalytics-commonobj.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C008052C-36A0-433E-A971-D1B8E499BF71}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{73482196-F29F-41F5-BA9A-A18108D68A10}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="HomeLandingTopicCards" sheetId="10" r:id="rId1"/>
-    <sheet name="MegaMenuInfo" sheetId="11" r:id="rId2"/>
-    <sheet name="TimingScroll" sheetId="12" r:id="rId3"/>
+    <sheet name="HomePageCards" sheetId="13" r:id="rId1"/>
+    <sheet name="LandingPageCards" sheetId="14" r:id="rId2"/>
+    <sheet name="MegaMenuInfo" sheetId="11" r:id="rId3"/>
+    <sheet name="TimingScroll" sheetId="12" r:id="rId4"/>
+    <sheet name="TopicPageCards" sheetId="15" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="50">
   <si>
     <t>Path</t>
   </si>
@@ -35,48 +37,27 @@
     <t>ContentType</t>
   </si>
   <si>
-    <t>CardPos</t>
-  </si>
-  <si>
     <t>/</t>
   </si>
   <si>
-    <t>Home</t>
-  </si>
-  <si>
-    <t>CardType</t>
-  </si>
-  <si>
     <t>LinkSelector</t>
   </si>
   <si>
     <t>TitleSelector</t>
   </si>
   <si>
-    <t>Feature</t>
-  </si>
-  <si>
     <t>.feature-primary .feature-card h3</t>
   </si>
   <si>
-    <t>Guide</t>
-  </si>
-  <si>
     <t>.guide-card .card h2</t>
   </si>
   <si>
     <t>.multimedia div[class*=feature-card] h3</t>
   </si>
   <si>
-    <t>Multimedia</t>
-  </si>
-  <si>
     <t>.guide-card .card h2  + ul li a</t>
   </si>
   <si>
-    <t>Thumbnail</t>
-  </si>
-  <si>
     <t>.card-thumbnail h3 a</t>
   </si>
   <si>
@@ -86,30 +67,18 @@
     <t>/about-cancer</t>
   </si>
   <si>
-    <t>SecondaryFeature</t>
-  </si>
-  <si>
     <t>.feature-secondary .feature-card h3</t>
   </si>
   <si>
     <t>/about-nci/organization/crchd</t>
   </si>
   <si>
-    <t>SlottedTopicCard</t>
-  </si>
-  <si>
-    <t>Topic</t>
-  </si>
-  <si>
     <t>.topic-feature .feature-card a h3</t>
   </si>
   <si>
     <t>/about-cancer/treatment</t>
   </si>
   <si>
-    <t>InlineCard</t>
-  </si>
-  <si>
     <t>#cgvBody .feature-card a h3</t>
   </si>
   <si>
@@ -174,6 +143,42 @@
   </si>
   <si>
     <t>Article</t>
+  </si>
+  <si>
+    <t>CardTypePosition</t>
+  </si>
+  <si>
+    <t>Feature:1</t>
+  </si>
+  <si>
+    <t>Guide:1</t>
+  </si>
+  <si>
+    <t>Multimedia:2</t>
+  </si>
+  <si>
+    <t>Thumbnail:1</t>
+  </si>
+  <si>
+    <t>SecondaryFeature:3</t>
+  </si>
+  <si>
+    <t>InlineCard:1</t>
+  </si>
+  <si>
+    <t>SlottedTopicCard:1</t>
+  </si>
+  <si>
+    <t>Multimedia:1</t>
+  </si>
+  <si>
+    <t>/research</t>
+  </si>
+  <si>
+    <t>Feature:2</t>
+  </si>
+  <si>
+    <t>Thumbnail:2</t>
   </si>
 </sst>
 </file>
@@ -223,12 +228,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,294 +546,232 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F2B56E1-BA35-4071-8CAC-1CCCC51E0A7D}">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B1045D-7223-4887-961C-26C884DD6A7F}">
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="37" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
+      <c r="D7" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF5B4D7-78BB-4A10-8C30-853138B87B32}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0546EB62-9EAA-40B6-9895-47102C6D888C}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,67 +787,67 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -913,11 +855,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3684BF6F-55B7-48F3-883C-A89530045D73}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -937,26 +879,102 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01929DA8-F50A-4B25-9225-A16CFAB01B23}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>